<commit_message>
Fix: Corriger téléchargement template Excel et ajouter lien Profils de Format
- Supprimer la documentation inutile (Documentation_Format_Standard.md)
- Régénérer le fichier Excel template pour corriger la corruption
- Retirer le lien vers la documentation dans TrancheWizard
- Ajouter section "Outils avancés" dans AdminPanel pour super admins
- Ajouter lien vers /admin/profils-format dans le panneau admin
- Importer FileSpreadsheet icon dans AdminPanel
- Corriger erreurs ESLint (unused vars, any types)
</commit_message>
<xml_diff>
--- a/public/templates/Modele_Registre_Titres.xlsx
+++ b/public/templates/Modele_Registre_Titres.xlsx
@@ -1111,7 +1111,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="bVNBmvENMjOt4Fbf4vGAXkU9mO6keGuCB/RMk9i4S3lLmQElCh/1gKPdvPSyRR0FUkfJOrs7pwuZaVvotodJtg==" saltValue="JDmlfUSHrjN+qDv+Jk7Phg==" spinCount="100000"/>
+  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="CZhEBXNvzDVn4+J3ZPuhkumzGewvoLGwteP09uGbegQ2AfWJ5ihNjOiyMdsfdkT9MDspc8o7QJmsoEocvXM60w==" saltValue="HRO34n77rao/cG/sWLYkgg==" spinCount="100000"/>
   <mergeCells count="1">
     <mergeCell ref="A1:A3"/>
   </mergeCells>
@@ -2265,7 +2265,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="7TSNR8qQ5XZsoYQG5mkjG4CnTjC45N/1c0spClj04wpDSHLZa9yV+26SmrehayqTjUeW0yZ34SQmwkuu8MRjWw==" saltValue="pxDlbT1nEQI4rs7ry1uE7g==" spinCount="100000"/>
+  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="HaCsHs54Lmw2lR8byK8Z1Gi2OAuUlT63eP4oLVUMykzVu0+/jwR9L+Ujs9tgr7cTwrk7VQhY2joQzKGQe2KqRw==" saltValue="6TaxuCgmSClAmnZ4XnZ1rw==" spinCount="100000"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Fix Excel template corruption issue
- Simplified template generator to avoid overlapping data validations
- Reduced validation count from 116 to 12 (only dropdowns)
- Removed input messages that were causing conflicts
- Template now opens correctly in Microsoft Excel
</commit_message>
<xml_diff>
--- a/public/templates/Modele_Registre_Titres.xlsx
+++ b/public/templates/Modele_Registre_Titres.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>Personnes Physiques</t>
   </si>
@@ -183,10 +183,7 @@
     <t>Client Professionnel</t>
   </si>
   <si>
-    <t>GUIDE D'UTILISATION</t>
-  </si>
-  <si>
-    <t>ETAPES</t>
+    <t>ETAPES:</t>
   </si>
   <si>
     <t>1. Allez sur l'onglet "Registre" (premier onglet)</t>
@@ -198,194 +195,65 @@
     <t>3. Remplissez la section "Personnes Morales" pour les entreprises</t>
   </si>
   <si>
-    <t>4. Supprimez les lignes "EXEMPLE" avant l'import (ou laissez-les, elles seront ignorees)</t>
-  </si>
-  <si>
-    <t>5. Enregistrez le fichier et importez-le dans Finixar</t>
-  </si>
-  <si>
-    <t>COLONNES</t>
-  </si>
-  <si>
-    <t>Les colonnes sur fond BLEU sont OBLIGATOIRES - vous devez les remplir</t>
-  </si>
-  <si>
-    <t>Les colonnes sur fond GRIS sont OPTIONNELLES - remplissez-les si vous avez l'information</t>
-  </si>
-  <si>
-    <t>Les lignes JAUNES sont des exemples - elles ne seront pas importees</t>
-  </si>
-  <si>
-    <t>FORMATS ATTENDUS</t>
-  </si>
-  <si>
-    <t>Dates: jj/mm/aaaa (exemple: 15/03/1980)</t>
-  </si>
-  <si>
-    <t>E-mail: format valide avec @ (exemple: nom@domaine.fr)</t>
-  </si>
-  <si>
-    <t>SIREN: exactement 9 chiffres (exemple: 123456789)</t>
-  </si>
-  <si>
-    <t>Telephone: avec ou sans indicatif (exemple: +33612345678 ou 0612345678)</t>
-  </si>
-  <si>
-    <t>Montants: nombres (exemple: 10000 ou 10000.50)</t>
-  </si>
-  <si>
-    <t>CONSEILS</t>
-  </si>
-  <si>
-    <t>Utilisez les listes deroulantes quand elles sont disponibles (PPE, Categorisation, etc.)</t>
-  </si>
-  <si>
-    <t>Survolez les en-tetes de colonnes pour voir les explications</t>
-  </si>
-  <si>
-    <t>Ne modifiez pas les en-tetes de colonnes</t>
-  </si>
-  <si>
-    <t>Gardez la structure avec les deux sections separees</t>
-  </si>
-  <si>
-    <t>SUPPORT</t>
-  </si>
-  <si>
-    <t>En cas de probleme, contactez le support Finixar</t>
-  </si>
-  <si>
-    <t>Consultez la documentation en ligne pour plus de details</t>
-  </si>
-  <si>
-    <t>DICTIONNAIRE DES CHAMPS</t>
-  </si>
-  <si>
-    <t>Champ</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Obligatoire</t>
-  </si>
-  <si>
-    <t>PERSONNES PHYSIQUES</t>
-  </si>
-  <si>
-    <t>Nombre d'obligations souscrites (nombre entier)</t>
-  </si>
-  <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Montant total investi en euros</t>
-  </si>
-  <si>
-    <t>Nom(s) de famille de l'investisseur</t>
-  </si>
-  <si>
-    <t>Prénom(s) de l'investisseur</t>
-  </si>
-  <si>
-    <t>Adresse e-mail valide</t>
-  </si>
-  <si>
-    <t>Format: +33612345678 ou 0612345678</t>
-  </si>
-  <si>
-    <t>Date de naissance (jj/mm/aaaa)</t>
-  </si>
-  <si>
-    <t>Ville de naissance</t>
-  </si>
-  <si>
-    <t>Numéro du département</t>
-  </si>
-  <si>
-    <t>Adresse complète</t>
-  </si>
-  <si>
-    <t>Pays de résidence fiscale</t>
-  </si>
-  <si>
-    <t>Personne Politiquement Exposée</t>
-  </si>
-  <si>
-    <t>Catégorie MiFID</t>
-  </si>
-  <si>
-    <t>Date de souscription (jj/mm/aaaa)</t>
-  </si>
-  <si>
-    <t>Nom d'usage si différent</t>
-  </si>
-  <si>
-    <t>Date de validation back-office</t>
-  </si>
-  <si>
-    <t>Compte PEA actif</t>
-  </si>
-  <si>
-    <t>Numéro du compte PEA si applicable</t>
-  </si>
-  <si>
-    <t>Nom du Conseiller en Gestion de Patrimoine</t>
-  </si>
-  <si>
-    <t>Code identifiant du CGP</t>
-  </si>
-  <si>
-    <t>SIREN du CGP (9 chiffres)</t>
-  </si>
-  <si>
-    <t>PERSONNES MORALES</t>
-  </si>
-  <si>
-    <t>Nombre d'obligations souscrites</t>
-  </si>
-  <si>
-    <t>Dénomination sociale de l'entreprise</t>
-  </si>
-  <si>
-    <t>Numéro SIREN (exactement 9 chiffres)</t>
-  </si>
-  <si>
-    <t>Prénom du représentant</t>
-  </si>
-  <si>
-    <t>Nom du représentant</t>
-  </si>
-  <si>
-    <t>Téléphone de l'entreprise</t>
-  </si>
-  <si>
-    <t>Adresse complète du siège</t>
-  </si>
-  <si>
-    <t>Pays de résidence fiscale du représentant</t>
-  </si>
-  <si>
-    <t>Représentant Politiquement Exposé</t>
-  </si>
-  <si>
-    <t>Compte PEA-PME actif</t>
-  </si>
-  <si>
-    <t>Numéro du compte si applicable</t>
-  </si>
-  <si>
-    <t>Conseiller en Gestion de Patrimoine</t>
-  </si>
-  <si>
-    <t>SIREN du CGP</t>
+    <t>4. Les lignes jaunes "EXEMPLE" seront ignorées lors de l'import</t>
+  </si>
+  <si>
+    <t>5. Enregistrez et importez le fichier dans Finixar</t>
+  </si>
+  <si>
+    <t>COLONNES:</t>
+  </si>
+  <si>
+    <t>- Fond BLEU/VERT = OBLIGATOIRE</t>
+  </si>
+  <si>
+    <t>- Fond GRIS = OPTIONNEL</t>
+  </si>
+  <si>
+    <t>- Fond JAUNE = Exemple (ignoré)</t>
+  </si>
+  <si>
+    <t>FORMATS:</t>
+  </si>
+  <si>
+    <t>- Dates: jj/mm/aaaa (ex: 15/03/1980)</t>
+  </si>
+  <si>
+    <t>- E-mail: format valide avec @</t>
+  </si>
+  <si>
+    <t>- SIREN: exactement 9 chiffres</t>
+  </si>
+  <si>
+    <t>- Téléphone: +33612345678 ou 0612345678</t>
+  </si>
+  <si>
+    <t>CONSEILS:</t>
+  </si>
+  <si>
+    <t>- Utilisez les listes déroulantes (PPE, Catégorisation, etc.)</t>
+  </si>
+  <si>
+    <t>- Ne modifiez pas les en-têtes de colonnes</t>
+  </si>
+  <si>
+    <t>- Gardez les deux sections séparées</t>
+  </si>
+  <si>
+    <t>CHAMPS OBLIGATOIRES</t>
+  </si>
+  <si>
+    <t>Personnes Physiques:</t>
+  </si>
+  <si>
+    <t>Personnes Morales:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -430,32 +298,21 @@
     <font>
       <b/>
       <color rgb="FF1E40AF"/>
-      <sz val="13"/>
     </font>
     <font>
       <b/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <b/>
+      <sz val="14"/>
     </font>
     <font>
       <b/>
       <color rgb="FF2563EB"/>
     </font>
     <font>
-      <color rgb="FF059669"/>
-    </font>
-    <font>
-      <color rgb="FF6B7280"/>
-    </font>
-    <font>
       <b/>
       <color rgb="FF059669"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,18 +374,8 @@
         <fgColor rgb="FF10B981"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8FAFC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBBF24"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -536,56 +383,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFCD34D"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFCD34D"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFCD34D"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFCD34D"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFE5E7EB"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFE5E7EB"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFE5E7EB"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFE5E7EB"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,39 +398,30 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,11 +1647,11 @@
       </c>
     </row>
     <row r="31" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -1877,11 +1670,11 @@
       <c r="U31" s="8"/>
     </row>
     <row r="32" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -1900,11 +1693,11 @@
       <c r="U32" s="8"/>
     </row>
     <row r="33" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -1923,11 +1716,11 @@
       <c r="U33" s="8"/>
     </row>
     <row r="34" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -1946,11 +1739,11 @@
       <c r="U34" s="8"/>
     </row>
     <row r="35" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
@@ -1969,11 +1762,11 @@
       <c r="U35" s="8"/>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
@@ -1992,11 +1785,11 @@
       <c r="U36" s="8"/>
     </row>
     <row r="37" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -2015,11 +1808,11 @@
       <c r="U37" s="8"/>
     </row>
     <row r="38" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -2038,11 +1831,11 @@
       <c r="U38" s="8"/>
     </row>
     <row r="39" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
@@ -2061,11 +1854,11 @@
       <c r="U39" s="8"/>
     </row>
     <row r="40" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -2084,11 +1877,11 @@
       <c r="U40" s="8"/>
     </row>
     <row r="41" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -2107,11 +1900,11 @@
       <c r="U41" s="8"/>
     </row>
     <row r="42" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
@@ -2130,11 +1923,11 @@
       <c r="U42" s="8"/>
     </row>
     <row r="43" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
@@ -2153,11 +1946,11 @@
       <c r="U43" s="8"/>
     </row>
     <row r="44" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
@@ -2176,11 +1969,11 @@
       <c r="U44" s="8"/>
     </row>
     <row r="45" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
@@ -2199,11 +1992,11 @@
       <c r="U45" s="8"/>
     </row>
     <row r="46" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
@@ -2222,11 +2015,11 @@
       <c r="U46" s="8"/>
     </row>
     <row r="47" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -2245,11 +2038,11 @@
       <c r="U47" s="8"/>
     </row>
     <row r="48" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -2268,11 +2061,11 @@
       <c r="U48" s="8"/>
     </row>
     <row r="49" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
@@ -2291,11 +2084,11 @@
       <c r="U49" s="8"/>
     </row>
     <row r="50" ht="22" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
@@ -2322,163 +2115,43 @@
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="F28:V28"/>
   </mergeCells>
-  <dataValidations count="116">
-    <dataValidation showInputMessage="1" promptTitle="Quantité" prompt="Nombre d'obligations souscrites (nombre entier)" sqref="A10:A24"/>
-    <dataValidation showInputMessage="1" promptTitle="Quantité" prompt="Nombre d'obligations souscrites" sqref="A29"/>
-    <dataValidation showInputMessage="1" promptTitle="Quantité" prompt="Nombre d'obligations souscrites (nombre entier)" sqref="A3"/>
-    <dataValidation showInputMessage="1" promptTitle="Quantité" prompt="Nombre d'obligations souscrites" sqref="A31:A50"/>
-    <dataValidation showInputMessage="1" promptTitle="Quantité" prompt="Nombre d'obligations souscrites (nombre entier)" sqref="A5:A24"/>
-    <dataValidation showInputMessage="1" promptTitle="Montant" prompt="Montant total investi en euros" sqref="B10:B24"/>
-    <dataValidation showInputMessage="1" promptTitle="Montant" prompt="Montant total investi en euros" sqref="B29"/>
-    <dataValidation showInputMessage="1" promptTitle="Montant" prompt="Montant total investi en euros" sqref="B3"/>
-    <dataValidation showInputMessage="1" promptTitle="Montant" prompt="Montant total investi en euros" sqref="B31:B50"/>
-    <dataValidation showInputMessage="1" promptTitle="Montant" prompt="Montant total investi en euros" sqref="B5:B24"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom(s)" prompt="Nom(s) de famille de l'investisseur" sqref="C10:C24"/>
-    <dataValidation showInputMessage="1" promptTitle="Raison sociale" prompt="Dénomination sociale de l'entreprise" sqref="C29"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom(s)" prompt="Nom(s) de famille de l'investisseur" sqref="C3"/>
-    <dataValidation showInputMessage="1" promptTitle="Raison sociale" prompt="Dénomination sociale de l'entreprise" sqref="C31:C50"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom(s)" prompt="Nom(s) de famille de l'investisseur" sqref="C5:C24"/>
-    <dataValidation showInputMessage="1" promptTitle="Prénom(s)" prompt="Prénom(s) de l'investisseur" sqref="D10:D24"/>
-    <dataValidation showInputMessage="1" promptTitle="N° SIREN" prompt="Numéro SIREN (exactement 9 chiffres)" sqref="D29"/>
-    <dataValidation showInputMessage="1" promptTitle="Prénom(s)" prompt="Prénom(s) de l'investisseur" sqref="D3"/>
-    <dataValidation showInputMessage="1" promptTitle="N° SIREN" prompt="Numéro SIREN (exactement 9 chiffres)" sqref="D31:D50"/>
-    <dataValidation showInputMessage="1" promptTitle="Prénom(s)" prompt="Prénom(s) de l'investisseur" sqref="D5:D24"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail" prompt="Adresse e-mail valide" sqref="E10:E24"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du représentant légal" prompt="E-mail du représentant légal" sqref="E29"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail" prompt="Adresse e-mail valide" sqref="E3"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du représentant légal" prompt="E-mail du représentant légal" sqref="E31:E50"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail" prompt="Adresse e-mail valide" sqref="E5:E24"/>
-    <dataValidation showInputMessage="1" promptTitle="Téléphone" prompt="Format: +33612345678 ou 0612345678" sqref="F10:F24"/>
-    <dataValidation showInputMessage="1" promptTitle="Prénom du représentant légal" prompt="Prénom du représentant" sqref="F29"/>
-    <dataValidation showInputMessage="1" promptTitle="Téléphone" prompt="Format: +33612345678 ou 0612345678" sqref="F3"/>
-    <dataValidation showInputMessage="1" promptTitle="Prénom du représentant légal" prompt="Prénom du représentant" sqref="F31:F50"/>
-    <dataValidation showInputMessage="1" promptTitle="Téléphone" prompt="Format: +33612345678 ou 0612345678" sqref="F5:F24"/>
-    <dataValidation showInputMessage="1" promptTitle="Né(e) le" prompt="Date de naissance (jj/mm/aaaa)" sqref="G10:G24"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom du représentant légal" prompt="Nom du représentant" sqref="G29"/>
-    <dataValidation showInputMessage="1" promptTitle="Né(e) le" prompt="Date de naissance (jj/mm/aaaa)" sqref="G3"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom du représentant légal" prompt="Nom du représentant" sqref="G31:G50"/>
-    <dataValidation showInputMessage="1" promptTitle="Né(e) le" prompt="Date de naissance (jj/mm/aaaa)" sqref="G5:G24"/>
-    <dataValidation showInputMessage="1" promptTitle="Lieu de naissance" prompt="Ville de naissance" sqref="H10:H24"/>
-    <dataValidation showInputMessage="1" promptTitle="Téléphone" prompt="Téléphone de l'entreprise" sqref="H29"/>
-    <dataValidation showInputMessage="1" promptTitle="Lieu de naissance" prompt="Ville de naissance" sqref="H3"/>
-    <dataValidation showInputMessage="1" promptTitle="Téléphone" prompt="Téléphone de l'entreprise" sqref="H31:H50"/>
-    <dataValidation showInputMessage="1" promptTitle="Lieu de naissance" prompt="Ville de naissance" sqref="H5:H24"/>
-    <dataValidation showInputMessage="1" promptTitle="Département de naissance" prompt="Numéro du département" sqref="I10:I24"/>
-    <dataValidation showInputMessage="1" promptTitle="Adresse du siège social" prompt="Adresse complète du siège" sqref="I29"/>
-    <dataValidation showInputMessage="1" promptTitle="Département de naissance" prompt="Numéro du département" sqref="I3"/>
-    <dataValidation showInputMessage="1" promptTitle="Adresse du siège social" prompt="Adresse complète du siège" sqref="I31:I50"/>
-    <dataValidation showInputMessage="1" promptTitle="Département de naissance" prompt="Numéro du département" sqref="I5:I24"/>
-    <dataValidation showInputMessage="1" promptTitle="Adresse du domicile" prompt="Adresse complète" sqref="J10:J24"/>
-    <dataValidation showInputMessage="1" promptTitle="Résidence Fiscale 1 du représentant légal" prompt="Pays de résidence fiscale du représentant" sqref="J29"/>
-    <dataValidation showInputMessage="1" promptTitle="Adresse du domicile" prompt="Adresse complète" sqref="J3"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: France, Belgique, Suisse, Luxembourg, Autre" sqref="J30">
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" sqref="J30:J50">
       <formula1>"France,Belgique,Suisse,Luxembourg,Autre"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Résidence Fiscale 1 du représentant légal" prompt="Pays de résidence fiscale du représentant" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: France, Belgique, Suisse, Luxembourg, Autre" sqref="J31:J50">
+    <dataValidation type="list" allowBlank="1" sqref="K10:K24">
       <formula1>"France,Belgique,Suisse,Luxembourg,Autre"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Adresse du domicile" prompt="Adresse complète" sqref="J5:J24"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Résidence Fiscale 1" prompt="Pays de résidence fiscale" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: France, Belgique, Suisse, Luxembourg, Autre" sqref="K10:K24">
+    <dataValidation type="list" allowBlank="1" sqref="K4:K24">
       <formula1>"France,Belgique,Suisse,Luxembourg,Autre"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Département de naissance du représentant" prompt="Département de naissance du représentant" sqref="K29"/>
-    <dataValidation showInputMessage="1" promptTitle="Résidence Fiscale 1" prompt="Pays de résidence fiscale" sqref="K3"/>
-    <dataValidation showInputMessage="1" promptTitle="Département de naissance du représentant" prompt="Département de naissance du représentant" sqref="K31:K50"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: France, Belgique, Suisse, Luxembourg, Autre" sqref="K4">
-      <formula1>"France,Belgique,Suisse,Luxembourg,Autre"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Résidence Fiscale 1" prompt="Pays de résidence fiscale" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: France, Belgique, Suisse, Luxembourg, Autre" sqref="K5:K24">
-      <formula1>"France,Belgique,Suisse,Luxembourg,Autre"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="PPE" prompt="Personne Politiquement Exposée" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="L10:L24">
+    <dataValidation type="list" allowBlank="1" sqref="L10:L24">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="PPE" prompt="Représentant Politiquement Exposé" sqref="L29"/>
-    <dataValidation showInputMessage="1" promptTitle="PPE" prompt="Personne Politiquement Exposée" sqref="L3"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="L30">
+    <dataValidation type="list" allowBlank="1" sqref="L30:L50">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="PPE" prompt="Représentant Politiquement Exposé" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="L31:L50">
+    <dataValidation type="list" allowBlank="1" sqref="L4:L24">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="L4">
+    <dataValidation type="list" allowBlank="1" sqref="M10:M24">
+      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="M30:M50">
+      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="M4:M24">
+      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="P30:P50">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="PPE" prompt="Personne Politiquement Exposée" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="L5:L24">
+    <dataValidation type="list" allowBlank="1" sqref="Q10:Q24">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Catégorisation" prompt="Catégorie MiFID" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Client Professionnel, Client Non Professionnel, Contrepartie Éligible" sqref="M10:M24">
-      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Catégorisation" prompt="Catégorie MiFID" sqref="M29"/>
-    <dataValidation showInputMessage="1" promptTitle="Catégorisation" prompt="Catégorie MiFID" sqref="M3"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Client Professionnel, Client Non Professionnel, Contrepartie Éligible" sqref="M30">
-      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Catégorisation" prompt="Catégorie MiFID" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Client Professionnel, Client Non Professionnel, Contrepartie Éligible" sqref="M31:M50">
-      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Client Professionnel, Client Non Professionnel, Contrepartie Éligible" sqref="M4">
-      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Catégorisation" prompt="Catégorie MiFID" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Client Professionnel, Client Non Professionnel, Contrepartie Éligible" sqref="M5:M24">
-      <formula1>"Client Professionnel,Client Non Professionnel,Contrepartie Éligible"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Date de Transfert" prompt="Date de souscription (jj/mm/aaaa)" sqref="N10:N24"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Transfert" prompt="Date de souscription (jj/mm/aaaa)" sqref="N29"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Transfert" prompt="Date de souscription (jj/mm/aaaa)" sqref="N3"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Transfert" prompt="Date de souscription (jj/mm/aaaa)" sqref="N31:N50"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Transfert" prompt="Date de souscription (jj/mm/aaaa)" sqref="N5:N24"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom d'usage" prompt="Nom d'usage si différent" sqref="O10:O24"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Validation BS" prompt="Date de validation back-office" sqref="O29"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom d'usage" prompt="Nom d'usage si différent" sqref="O3"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Validation BS" prompt="Date de validation back-office" sqref="O31:O50"/>
-    <dataValidation showInputMessage="1" promptTitle="Nom d'usage" prompt="Nom d'usage si différent" sqref="O5:O24"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Validation BS" prompt="Date de validation back-office" sqref="P10:P24"/>
-    <dataValidation showInputMessage="1" promptTitle="PEA / PEA-PME" prompt="Compte PEA-PME actif" sqref="P29"/>
-    <dataValidation showInputMessage="1" promptTitle="Date de Validation BS" prompt="Date de validation back-office" sqref="P3"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="P30">
+    <dataValidation type="list" allowBlank="1" sqref="Q4:Q24">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="PEA / PEA-PME" prompt="Compte PEA-PME actif" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="P31:P50">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Date de Validation BS" prompt="Date de validation back-office" sqref="P5:P24"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="PEA / PEA-PME" prompt="Compte PEA actif" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="Q10:Q24">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Numéro de Compte PEA / PEA-PME" prompt="Numéro du compte si applicable" sqref="Q29"/>
-    <dataValidation showInputMessage="1" promptTitle="PEA / PEA-PME" prompt="Compte PEA actif" sqref="Q3"/>
-    <dataValidation showInputMessage="1" promptTitle="Numéro de Compte PEA / PEA-PME" prompt="Numéro du compte si applicable" sqref="Q31:Q50"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="Q4">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="PEA / PEA-PME" prompt="Compte PEA actif" showErrorMessage="1" errorTitle="Valeur invalide" error="Veuillez choisir parmi: Oui, Non" sqref="Q5:Q24">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="Numéro de Compte PEA / PEA-PME" prompt="Numéro du compte PEA si applicable" sqref="R10:R24"/>
-    <dataValidation showInputMessage="1" promptTitle="CGP" prompt="Conseiller en Gestion de Patrimoine" sqref="R29"/>
-    <dataValidation showInputMessage="1" promptTitle="Numéro de Compte PEA / PEA-PME" prompt="Numéro du compte PEA si applicable" sqref="R3"/>
-    <dataValidation showInputMessage="1" promptTitle="CGP" prompt="Conseiller en Gestion de Patrimoine" sqref="R31:R50"/>
-    <dataValidation showInputMessage="1" promptTitle="Numéro de Compte PEA / PEA-PME" prompt="Numéro du compte PEA si applicable" sqref="R5:R24"/>
-    <dataValidation showInputMessage="1" promptTitle="CGP" prompt="Nom du Conseiller en Gestion de Patrimoine" sqref="S10:S24"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du CGP" prompt="E-mail du CGP" sqref="S29"/>
-    <dataValidation showInputMessage="1" promptTitle="CGP" prompt="Nom du Conseiller en Gestion de Patrimoine" sqref="S3"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du CGP" prompt="E-mail du CGP" sqref="S31:S50"/>
-    <dataValidation showInputMessage="1" promptTitle="CGP" prompt="Nom du Conseiller en Gestion de Patrimoine" sqref="S5:S24"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du CGP" prompt="E-mail du CGP" sqref="T10:T24"/>
-    <dataValidation showInputMessage="1" promptTitle="Code du CGP" prompt="Code du CGP" sqref="T29"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du CGP" prompt="E-mail du CGP" sqref="T3"/>
-    <dataValidation showInputMessage="1" promptTitle="Code du CGP" prompt="Code du CGP" sqref="T31:T50"/>
-    <dataValidation showInputMessage="1" promptTitle="E-mail du CGP" prompt="E-mail du CGP" sqref="T5:T24"/>
-    <dataValidation showInputMessage="1" promptTitle="Code du CGP" prompt="Code identifiant du CGP" sqref="U10:U24"/>
-    <dataValidation showInputMessage="1" promptTitle="Siren du CGP" prompt="SIREN du CGP" sqref="U29"/>
-    <dataValidation showInputMessage="1" promptTitle="Code du CGP" prompt="Code identifiant du CGP" sqref="U3"/>
-    <dataValidation showInputMessage="1" promptTitle="Siren du CGP" prompt="SIREN du CGP" sqref="U31:U50"/>
-    <dataValidation showInputMessage="1" promptTitle="Code du CGP" prompt="Code identifiant du CGP" sqref="U5:U24"/>
-    <dataValidation showInputMessage="1" promptTitle="Siren du CGP" prompt="SIREN du CGP (9 chiffres)" sqref="V10:V24"/>
-    <dataValidation showInputMessage="1" promptTitle="Siren du CGP" prompt="SIREN du CGP (9 chiffres)" sqref="V3"/>
-    <dataValidation showInputMessage="1" promptTitle="Siren du CGP" prompt="SIREN du CGP (9 chiffres)" sqref="V5:V24"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -2490,43 +2163,50 @@
   <sheetPr>
     <tabColor rgb="FF2563EB"/>
   </sheetPr>
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A23"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="80" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>57</v>
+      <c r="A4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>58</v>
+      <c r="A5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>59</v>
+      <c r="A6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>60</v>
+      <c r="A7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>61</v>
+      <c r="A8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -2534,19 +2214,24 @@
         <v>62</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>63</v>
+      <c r="A11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>64</v>
+      <c r="A12" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>65</v>
+      <c r="A13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -2554,24 +2239,29 @@
         <v>66</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>67</v>
+      <c r="A16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>68</v>
+      <c r="A17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>69</v>
+      <c r="A18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>70</v>
+      <c r="A19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -2580,55 +2270,21 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="BrCOYZoYtL9McfH1tQ0UanFf09PAf9q13XNM9pZ1kk1J+FyMGsaPZdrkah3fq4lYcmmAyNE7xIWe90sBQHvTIw==" saltValue="D4E2aIbMr0O2mvO5df3OEw==" spinCount="100000"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -2639,520 +2295,79 @@
   <sheetPr>
     <tabColor rgb="FFFBBF24"/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:A15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>35</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="dDIHhLkxevbqbn4BdvVb5xiO6EPLb5awWp0LWDq7J+aY6I9qb0v5xqqWsS32QcFyJF68VKWq7B3Ein+O3pcMIQ==" saltValue="Fnuh8RnpIIqIUp3yEyS+pw==" spinCount="100000"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize Excel template to include only imported fields
Remove unused columns from the tranche wizard Excel template:
- Physical persons: removed Nom d'usage, PPE, Catégorisation, Date de Validation BS, PEA/PEA-PME fields, Code/Siren du CGP
- Moral persons: removed Résidence Fiscale du représentant, PPE, Catégorisation, Date de Validation BS, PEA/PEA-PME fields, Code/Siren du CGP

These fields were in the template but never actually saved by the import function. Keeping only the 14 columns for physical persons and 13 for moral persons that are actually imported to the database.

https://claude.ai/code/session_01HugrCn8s3YfU1k3LgXHr7E
</commit_message>
<xml_diff>
--- a/public/templates/Modele_Registre_Titres.xlsx
+++ b/public/templates/Modele_Registre_Titres.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="118">
   <si>
     <t>📋 MODÈLE REGISTRE DES TITRES</t>
   </si>
@@ -60,19 +60,28 @@
     <t>• Nom(s), Prénom(s)</t>
   </si>
   <si>
-    <t>• E-mail</t>
+    <t>• E-mail, Téléphone</t>
+  </si>
+  <si>
+    <t>• Date de naissance, Lieu de naissance</t>
+  </si>
+  <si>
+    <t>• Adresse, Résidence Fiscale</t>
+  </si>
+  <si>
+    <t>• Date de Transfert</t>
   </si>
   <si>
     <t>Personnes Morales :</t>
   </si>
   <si>
-    <t>• Raison sociale</t>
-  </si>
-  <si>
-    <t>• N° SIREN (9 chiffres)</t>
-  </si>
-  <si>
-    <t>• E-mail du représentant légal</t>
+    <t>• Raison sociale, N° SIREN (9 chiffres)</t>
+  </si>
+  <si>
+    <t>• E-mail du représentant légal, Téléphone</t>
+  </si>
+  <si>
+    <t>• Adresse du siège social</t>
   </si>
   <si>
     <t>📐 Formats attendus</t>
@@ -84,15 +93,12 @@
     <t>• E-mail : doit contenir un @</t>
   </si>
   <si>
-    <t>• SIREN : exactement 9 chiffres</t>
+    <t>• SIREN : exactement 9 chiffres (personnes morales uniquement)</t>
   </si>
   <si>
     <t>• Téléphone : numéros avec ou sans +</t>
   </si>
   <si>
-    <t>• PPE : Oui ou Non</t>
-  </si>
-  <si>
     <t>• Montants : nombres décimaux acceptés</t>
   </si>
   <si>
@@ -117,9 +123,6 @@
     <t>Prénom(s) *</t>
   </si>
   <si>
-    <t>Nom d'usage</t>
-  </si>
-  <si>
     <t>E-mail *</t>
   </si>
   <si>
@@ -141,153 +144,108 @@
     <t>Résidence Fiscale 1 *</t>
   </si>
   <si>
-    <t>PPE *</t>
-  </si>
-  <si>
-    <t>Catégorisation *</t>
-  </si>
-  <si>
     <t>Date de Transfert *</t>
   </si>
   <si>
-    <t>Date de Validation BS</t>
-  </si>
-  <si>
-    <t>PEA / PEA-PME</t>
-  </si>
-  <si>
-    <t>Numéro de Compte PEA / PEA-PME</t>
-  </si>
-  <si>
     <t>CGP</t>
   </si>
   <si>
     <t>E-mail du CGP</t>
   </si>
   <si>
-    <t>Code du CGP</t>
-  </si>
-  <si>
-    <t>Siren du CGP</t>
-  </si>
-  <si>
     <t>Dupont</t>
   </si>
   <si>
     <t>Jean</t>
   </si>
   <si>
+    <t>jean.dupont@exemple.fr</t>
+  </si>
+  <si>
+    <t>+33612345678</t>
+  </si>
+  <si>
+    <t>15/03/1980</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>75 - Paris</t>
+  </si>
+  <si>
+    <t>123 Rue de la République, 75001 Paris</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>01/01/2024</t>
+  </si>
+  <si>
+    <t>Cabinet Dupuis</t>
+  </si>
+  <si>
+    <t>contact@cabinet-dupuis.fr</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>sophie.martin@exemple.fr</t>
+  </si>
+  <si>
+    <t>0687654321</t>
+  </si>
+  <si>
+    <t>22/07/1975</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>69 - Rhône</t>
+  </si>
+  <si>
+    <t>45 Avenue des Champs, 69001 Lyon</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>jean.dupont@exemple.fr</t>
-  </si>
-  <si>
-    <t>+33612345678</t>
-  </si>
-  <si>
-    <t>15/03/1980</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>75 - Paris</t>
-  </si>
-  <si>
-    <t>123 Rue de la République, 75001 Paris</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Non</t>
-  </si>
-  <si>
-    <t>Client Professionnel</t>
-  </si>
-  <si>
-    <t>01/01/2024</t>
-  </si>
-  <si>
-    <t>05/01/2024</t>
-  </si>
-  <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>PEA123456789</t>
-  </si>
-  <si>
-    <t>Cabinet Dupuis</t>
-  </si>
-  <si>
-    <t>contact@cabinet-dupuis.fr</t>
-  </si>
-  <si>
-    <t>CGP001</t>
+    <t>Personnes Morales</t>
+  </si>
+  <si>
+    <t>Raison sociale *</t>
+  </si>
+  <si>
+    <t>N° SIREN *</t>
+  </si>
+  <si>
+    <t>E-mail du représentant légal *</t>
+  </si>
+  <si>
+    <t>Prénom du représentant légal</t>
+  </si>
+  <si>
+    <t>Nom du représentant légal</t>
+  </si>
+  <si>
+    <t>Adresse du siège social *</t>
+  </si>
+  <si>
+    <t>Département de naissance du représentant</t>
+  </si>
+  <si>
+    <t>ACME Corporation</t>
   </si>
   <si>
     <t>123456789</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Sophie</t>
-  </si>
-  <si>
-    <t>sophie.martin@exemple.fr</t>
-  </si>
-  <si>
-    <t>0687654321</t>
-  </si>
-  <si>
-    <t>22/07/1975</t>
-  </si>
-  <si>
-    <t>Lyon</t>
-  </si>
-  <si>
-    <t>69 - Rhône</t>
-  </si>
-  <si>
-    <t>45 Avenue des Champs, 69001 Lyon</t>
-  </si>
-  <si>
-    <t>Client Non Professionnel</t>
-  </si>
-  <si>
-    <t>Personnes Morales</t>
-  </si>
-  <si>
-    <t>Raison sociale *</t>
-  </si>
-  <si>
-    <t>N° SIREN *</t>
-  </si>
-  <si>
-    <t>E-mail du représentant légal *</t>
-  </si>
-  <si>
-    <t>Prénom du représentant légal</t>
-  </si>
-  <si>
-    <t>Nom du représentant légal</t>
-  </si>
-  <si>
-    <t>Adresse du siège social *</t>
-  </si>
-  <si>
-    <t>Résidence Fiscale 1 du représentant légal</t>
-  </si>
-  <si>
-    <t>Département de naissance du représentant</t>
-  </si>
-  <si>
-    <t>ACME Corporation</t>
-  </si>
-  <si>
     <t>contact@acme-corp.fr</t>
   </si>
   <si>
@@ -303,24 +261,18 @@
     <t>10 Boulevard des Entreprises, 92000 Nanterre</t>
   </si>
   <si>
-    <t>Contrepartie Éligible</t>
-  </si>
-  <si>
     <t>Cabinet Finance Pro</t>
   </si>
   <si>
     <t>info@financepro.fr</t>
   </si>
   <si>
-    <t>CGP100</t>
+    <t>Tech Innovations SAS</t>
   </si>
   <si>
     <t>987654321</t>
   </si>
   <si>
-    <t>Tech Innovations SAS</t>
-  </si>
-  <si>
     <t>dirigeant@tech-innov.fr</t>
   </si>
   <si>
@@ -354,9 +306,6 @@
     <t>Prénom(s) de l'investisseur. Exemple : Jean</t>
   </si>
   <si>
-    <t>Nom d'usage si différent du nom de famille. Optionnel.</t>
-  </si>
-  <si>
     <t>Adresse e-mail valide. Doit contenir un @. Exemple : jean.dupont@exemple.fr</t>
   </si>
   <si>
@@ -378,22 +327,7 @@
     <t>Pays de résidence fiscale principal. Exemple : France</t>
   </si>
   <si>
-    <t>Personne Politiquement Exposée. Valeurs possibles : Oui ou Non</t>
-  </si>
-  <si>
-    <t>Catégorie MiFID. Exemples : Client Professionnel, Client Non Professionnel, Contrepartie Éligible</t>
-  </si>
-  <si>
-    <t>Date de transfert/souscription. Format : jj/mm/aaaa. Exemple : 01/01/2024</t>
-  </si>
-  <si>
-    <t>Date de validation par le back-office. Format : jj/mm/aaaa. Optionnel.</t>
-  </si>
-  <si>
-    <t>Compte PEA actif. Valeurs : Oui, Non, ou vide</t>
-  </si>
-  <si>
-    <t>Numéro du compte PEA si applicable. Optionnel.</t>
+    <t>Date de transfert/souscription (utilisée comme date d'émission). Format : jj/mm/aaaa. Exemple : 01/01/2024</t>
   </si>
   <si>
     <t>Nom du Conseiller en Gestion de Patrimoine. Optionnel.</t>
@@ -402,12 +336,6 @@
     <t>Adresse e-mail du CGP. Optionnel.</t>
   </si>
   <si>
-    <t>Code identifiant du CGP. Optionnel.</t>
-  </si>
-  <si>
-    <t>Numéro SIREN du CGP (9 chiffres). Optionnel.</t>
-  </si>
-  <si>
     <t>PERSONNES MORALES</t>
   </si>
   <si>
@@ -438,22 +366,7 @@
     <t>Adresse complète du siège social. Exemple : 10 Boulevard des Entreprises, 92000 Nanterre</t>
   </si>
   <si>
-    <t>Pays de résidence fiscale du représentant. Exemple : France</t>
-  </si>
-  <si>
     <t>Département de naissance du représentant légal. Exemple : 75 - Paris</t>
-  </si>
-  <si>
-    <t>Représentant Politiquement Exposé. Valeurs possibles : Oui ou Non</t>
-  </si>
-  <si>
-    <t>Catégorie MiFID. Exemples : Client Professionnel, Contrepartie Éligible</t>
-  </si>
-  <si>
-    <t>Compte PEA-PME actif. Valeurs : Oui, Non, ou vide</t>
-  </si>
-  <si>
-    <t>Numéro du compte PEA-PME si applicable. Optionnel.</t>
   </si>
 </sst>
 </file>
@@ -948,7 +861,7 @@
   <sheetPr>
     <tabColor rgb="FF2563EB"/>
   </sheetPr>
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A42"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="100" customWidth="1"/>
@@ -1040,78 +953,93 @@
         <v>15</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>16</v>
+      <c r="A23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
+      <c r="A26" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
+      <c r="A29" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="CZhEBXNvzDVn4+J3ZPuhkumzGewvoLGwteP09uGbegQ2AfWJ5ihNjOiyMdsfdkT9MDspc8o7QJmsoEocvXM60w==" saltValue="HRO34n77rao/cG/sWLYkgg==" spinCount="100000"/>
+  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="vx6ZXz+ABS2xgtaaiPuKM5GIBTrOnCqxM+gC9BirENh/laH3eFWgrscS9UGOvzTVfaKoU7YkPwPDVrnrtJ99Vw==" saltValue="/IchE7XKid4/cEaNT5W2vQ==" spinCount="100000"/>
   <mergeCells count="1">
     <mergeCell ref="A1:A3"/>
   </mergeCells>
@@ -1125,7 +1053,7 @@
   <sheetPr>
     <tabColor rgb="FF10B981"/>
   </sheetPr>
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:N30"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
@@ -1136,21 +1064,15 @@
     <col min="6" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="40" customWidth="1"/>
-    <col min="10" max="11" width="35" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="30" customWidth="1"/>
-    <col min="18" max="18" width="25" customWidth="1"/>
-    <col min="19" max="19" width="30" customWidth="1"/>
-    <col min="20" max="22" width="15" customWidth="1"/>
+    <col min="10" max="10" width="35" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="14" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1165,84 +1087,52 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>100</v>
       </c>
@@ -1250,67 +1140,43 @@
         <v>10000</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>50</v>
       </c>
@@ -1318,221 +1184,175 @@
         <v>5000</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="L4" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="12:13" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="12:13" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1546,82 +1366,49 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="N18" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O18" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="P18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="S18" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="T18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U18" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>500</v>
       </c>
@@ -1629,64 +1416,40 @@
         <v>50000</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="U19" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>200</v>
       </c>
@@ -1694,64 +1457,40 @@
         <v>20000</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="R20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="S20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1759,11 +1498,9 @@
       <c r="E21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1771,11 +1508,9 @@
       <c r="E22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -1783,11 +1518,9 @@
       <c r="E23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1795,11 +1528,9 @@
       <c r="E24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1807,11 +1538,9 @@
       <c r="E25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -1819,11 +1548,9 @@
       <c r="E26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1831,11 +1558,9 @@
       <c r="E27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1843,11 +1568,9 @@
       <c r="E28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -1855,11 +1578,9 @@
       <c r="E29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1867,26 +1588,13 @@
       <c r="E30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
+      <c r="K30" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="A17:V17"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A17:M17"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="L19:L30">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="M10:M14">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="M3:M14">
-      <formula1>"Oui,Non"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -1897,7 +1605,7 @@
   <sheetPr>
     <tabColor rgb="FFFBBF24"/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B33"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
@@ -1906,366 +1614,238 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>125</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>131</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="HaCsHs54Lmw2lR8byK8Z1Gi2OAuUlT63eP4oLVUMykzVu0+/jwR9L+Ujs9tgr7cTwrk7VQhY2joQzKGQe2KqRw==" saltValue="6TaxuCgmSClAmnZ4XnZ1rw==" spinCount="100000"/>
+  <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="ucoIm6PRZLyhIZoUhCuvFwaaMdGcmk+Jet94cIc5G4fzlU9rG+krvcTmW43j5QoGbERDP2KBlOWOhULZp2Yfbw==" saltValue="pu9JXkzKzVdkIXdkpzi8/w==" spinCount="100000"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>

</xml_diff>